<commit_message>
created emergency page on dashboard and updated the backlog
</commit_message>
<xml_diff>
--- a/doc/task11/scrum_v02.xlsx
+++ b/doc/task11/scrum_v02.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17024"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16440" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="19365" windowHeight="5865" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,8 @@
     <sheet name="Sprint Backlog" sheetId="3" r:id="rId3"/>
     <sheet name="BurndownChart" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171026" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
   <customWorkbookViews>
     <customWorkbookView name="Raphael Suter - Persönliche Ansicht" guid="{B138B3DD-F60C-400A-A386-DA8CE3FC6E3C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="855" activeSheetId="2"/>
   </customWorkbookViews>
@@ -375,8 +376,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -760,14 +761,14 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.350000000000001" customHeight="1">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -778,7 +779,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -789,7 +790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -800,7 +801,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -811,7 +812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -822,7 +823,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -852,7 +853,7 @@
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" style="7" customWidth="1"/>
@@ -864,7 +865,7 @@
     <col min="8" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="30">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -890,7 +891,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" ht="30">
+    <row r="2" spans="1:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -910,7 +911,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -930,7 +931,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="45">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -950,7 +951,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -970,7 +971,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -990,7 +991,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1010,7 +1011,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1030,7 +1031,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="45">
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1050,7 +1051,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="45">
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1070,7 +1071,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="60">
+    <row r="11" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1090,7 +1091,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1110,7 +1111,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="45">
+    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1130,7 +1131,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1150,7 +1151,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="45">
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1170,7 +1171,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="45">
+    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>99</v>
       </c>
@@ -1190,7 +1191,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30">
+    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1210,7 +1211,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="30">
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>98</v>
       </c>
@@ -1247,11 +1248,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" style="9" customWidth="1"/>
     <col min="2" max="2" width="6.140625" customWidth="1"/>
@@ -1267,7 +1268,7 @@
     <col min="12" max="12" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="44.25" customHeight="1">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>15</v>
       </c>
@@ -1305,7 +1306,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>65</v>
       </c>
@@ -1343,7 +1344,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="75">
+    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>71</v>
       </c>
@@ -1381,7 +1382,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="90">
+    <row r="4" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>74</v>
       </c>
@@ -1419,7 +1420,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="105">
+    <row r="5" spans="1:12" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>77</v>
       </c>
@@ -1454,7 +1455,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="30">
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>81</v>
       </c>
@@ -1483,7 +1484,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="30">
+    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>84</v>
       </c>
@@ -1518,7 +1519,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D8" s="7" t="s">
         <v>86</v>
       </c>
@@ -1532,7 +1533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30">
+    <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>87</v>
       </c>
@@ -1555,7 +1556,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>89</v>
       </c>
@@ -1578,7 +1579,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30">
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>91</v>
       </c>
@@ -1601,7 +1602,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>94</v>
       </c>
@@ -1624,7 +1625,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="30">
+    <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>95</v>
       </c>
@@ -1647,7 +1648,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="30">
+    <row r="14" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>98</v>
       </c>
@@ -1670,7 +1671,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>2</v>
       </c>
@@ -1690,7 +1691,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>2</v>
       </c>
@@ -1710,7 +1711,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="30">
+    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>102</v>
       </c>
@@ -1733,7 +1734,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>104</v>
       </c>
@@ -1752,11 +1753,14 @@
       <c r="I18">
         <v>1</v>
       </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
       <c r="L18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>2</v>
       </c>
@@ -1776,7 +1780,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>107</v>
       </c>
@@ -1796,7 +1800,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>109</v>
       </c>
@@ -1835,14 +1839,14 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.45" customHeight="1">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>111</v>
       </c>
@@ -1856,7 +1860,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1870,7 +1874,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>

</xml_diff>